<commit_message>
Mark the document as final
Add document signature
</commit_message>
<xml_diff>
--- a/docs/Banka KSD - QA Documentation.xlsx
+++ b/docs/Banka KSD - QA Documentation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maksm\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maksm\Documents\projects\banka-ksd\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11745"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11745" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Home menu" sheetId="2" r:id="rId1"/>
@@ -215,9 +215,6 @@
     <t>AI functionality</t>
   </si>
   <si>
-    <t>AI turn.</t>
-  </si>
-  <si>
     <t>TEST CASE 5</t>
   </si>
   <si>
@@ -291,6 +288,9 @@
   </si>
   <si>
     <t>Final status</t>
+  </si>
+  <si>
+    <t>AI turn</t>
   </si>
 </sst>
 </file>
@@ -499,56 +499,56 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -832,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:M66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,14 +846,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -861,12 +861,12 @@
       <c r="M1" s="3"/>
     </row>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -874,12 +874,12 @@
       <c r="M2" s="3"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -887,14 +887,14 @@
       <c r="M3" s="3"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -902,12 +902,12 @@
       <c r="M5" s="4"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -915,14 +915,14 @@
       <c r="M6" s="4"/>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -930,44 +930,44 @@
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="3:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
     </row>
     <row r="10" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
     </row>
     <row r="11" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C11" s="36"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
     </row>
     <row r="13" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C13" s="9" t="s">
@@ -1005,37 +1005,37 @@
       <c r="G14" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="37" t="s">
+      <c r="H14" s="22" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
     </row>
     <row r="22" spans="3:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="11" t="s">
@@ -1047,35 +1047,35 @@
       <c r="E22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="32" t="s">
+      <c r="F22" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="26" t="s">
+      <c r="F23" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="24"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C26" s="9" t="s">
@@ -1118,32 +1118,32 @@
       </c>
     </row>
     <row r="31" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
     </row>
     <row r="32" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
     </row>
     <row r="35" spans="3:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" s="11" t="s">
@@ -1155,35 +1155,35 @@
       <c r="E35" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F35" s="32" t="s">
+      <c r="F35" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="25"/>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="25" t="s">
+      <c r="D36" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E36" s="24" t="s">
+      <c r="E36" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F36" s="26" t="s">
+      <c r="F36" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C37" s="24"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C39" s="9" t="s">
@@ -1226,32 +1226,32 @@
       </c>
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C44" s="21" t="s">
+      <c r="C44" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="23"/>
     </row>
     <row r="45" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="21"/>
-      <c r="H45" s="21"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="23"/>
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C47" s="22" t="s">
+      <c r="C47" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D47" s="22"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="22"/>
-      <c r="G47" s="22"/>
-      <c r="H47" s="22"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="24"/>
     </row>
     <row r="48" spans="3:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C48" s="11" t="s">
@@ -1263,35 +1263,35 @@
       <c r="E48" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F48" s="32" t="s">
+      <c r="F48" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="G48" s="32"/>
-      <c r="H48" s="32"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="25"/>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C49" s="24" t="s">
+      <c r="C49" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D49" s="25" t="s">
+      <c r="D49" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E49" s="24" t="s">
+      <c r="E49" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="26" t="s">
+      <c r="F49" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
+      <c r="G49" s="28"/>
+      <c r="H49" s="28"/>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C50" s="24"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="26"/>
-      <c r="H50" s="26"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="28"/>
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C52" s="9" t="s">
@@ -1334,32 +1334,32 @@
       </c>
     </row>
     <row r="57" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C57" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="D57" s="21"/>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
-      <c r="G57" s="21"/>
-      <c r="H57" s="21"/>
+      <c r="C57" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="23"/>
+      <c r="H57" s="23"/>
     </row>
     <row r="58" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
-      <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
-      <c r="G58" s="21"/>
-      <c r="H58" s="21"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
+      <c r="H58" s="23"/>
     </row>
     <row r="60" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C60" s="22" t="s">
+      <c r="C60" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D60" s="22"/>
-      <c r="E60" s="22"/>
-      <c r="F60" s="22"/>
-      <c r="G60" s="22"/>
-      <c r="H60" s="22"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="24"/>
+      <c r="H60" s="24"/>
     </row>
     <row r="61" spans="3:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C61" s="17" t="s">
@@ -1371,35 +1371,35 @@
       <c r="E61" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F61" s="32" t="s">
+      <c r="F61" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="G61" s="32"/>
-      <c r="H61" s="32"/>
+      <c r="G61" s="25"/>
+      <c r="H61" s="25"/>
     </row>
     <row r="62" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C62" s="24" t="s">
+      <c r="C62" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D62" s="25" t="s">
+      <c r="D62" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E62" s="24" t="s">
+      <c r="E62" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F62" s="26" t="s">
+      <c r="F62" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G62" s="26"/>
-      <c r="H62" s="26"/>
+      <c r="G62" s="28"/>
+      <c r="H62" s="28"/>
     </row>
     <row r="63" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C63" s="24"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="24"/>
-      <c r="F63" s="26"/>
-      <c r="G63" s="26"/>
-      <c r="H63" s="26"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="27"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="28"/>
+      <c r="G63" s="28"/>
+      <c r="H63" s="28"/>
     </row>
     <row r="65" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C65" s="19" t="s">
@@ -1489,7 +1489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:M53"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="C44" sqref="C44:H45"/>
     </sheetView>
   </sheetViews>
@@ -1504,14 +1504,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -1519,12 +1519,12 @@
       <c r="M1" s="3"/>
     </row>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -1532,12 +1532,12 @@
       <c r="M2" s="3"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -1545,14 +1545,14 @@
       <c r="M3" s="3"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
+      <c r="C5" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -1560,12 +1560,12 @@
       <c r="M5" s="4"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -1573,14 +1573,14 @@
       <c r="M6" s="4"/>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -1588,44 +1588,44 @@
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="3:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
     </row>
     <row r="10" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
     </row>
     <row r="11" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C11" s="36"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
     </row>
     <row r="13" spans="3:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="6" t="s">
@@ -1663,37 +1663,37 @@
       <c r="G14" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H14" s="37" t="s">
+      <c r="H14" s="22" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C18" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
+      <c r="C18" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
     </row>
     <row r="22" spans="3:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="10" t="s">
@@ -1705,35 +1705,35 @@
       <c r="E22" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="32" t="s">
+      <c r="F22" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="26" t="s">
+      <c r="F23" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="24"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
     </row>
     <row r="26" spans="3:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="6" t="s">
@@ -1776,32 +1776,32 @@
       </c>
     </row>
     <row r="31" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C31" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
+      <c r="C31" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
     </row>
     <row r="32" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
     </row>
     <row r="35" spans="3:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" s="10" t="s">
@@ -1813,35 +1813,35 @@
       <c r="E35" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F35" s="32" t="s">
+      <c r="F35" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="25"/>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="25" t="s">
+      <c r="D36" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="E36" s="24" t="s">
+      <c r="E36" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F36" s="26" t="s">
+      <c r="F36" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C37" s="24"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
     </row>
     <row r="39" spans="3:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C39" s="6" t="s">
@@ -1884,32 +1884,32 @@
       </c>
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C44" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
+      <c r="C44" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="23"/>
     </row>
     <row r="45" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="21"/>
-      <c r="H45" s="21"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="23"/>
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C47" s="22" t="s">
+      <c r="C47" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D47" s="22"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="22"/>
-      <c r="G47" s="22"/>
-      <c r="H47" s="22"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="24"/>
     </row>
     <row r="48" spans="3:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C48" s="10" t="s">
@@ -1921,35 +1921,35 @@
       <c r="E48" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F48" s="32" t="s">
+      <c r="F48" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="G48" s="32"/>
-      <c r="H48" s="32"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="25"/>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C49" s="24" t="s">
+      <c r="C49" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D49" s="25" t="s">
+      <c r="D49" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="E49" s="24" t="s">
+      <c r="E49" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="26" t="s">
+      <c r="F49" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
+      <c r="G49" s="28"/>
+      <c r="H49" s="28"/>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C50" s="24"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="26"/>
-      <c r="H50" s="26"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="28"/>
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C52" s="6" t="s">
@@ -2032,8 +2032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:M66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2046,14 +2046,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -2061,12 +2061,12 @@
       <c r="M1" s="3"/>
     </row>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -2074,12 +2074,12 @@
       <c r="M2" s="3"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -2087,14 +2087,14 @@
       <c r="M3" s="3"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
+      <c r="C5" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -2102,12 +2102,12 @@
       <c r="M5" s="2"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -2115,14 +2115,14 @@
       <c r="M6" s="2"/>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -2130,44 +2130,44 @@
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="3:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
     </row>
     <row r="10" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
     </row>
     <row r="11" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="36"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
     </row>
     <row r="13" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C13" s="9" t="s">
@@ -2205,37 +2205,37 @@
       <c r="G14" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="H14" s="37" t="s">
+      <c r="H14" s="22" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C18" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
+      <c r="C18" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
     </row>
     <row r="21" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -2252,11 +2252,11 @@
       <c r="E22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="32" t="s">
+      <c r="F22" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -2264,28 +2264,28 @@
       <c r="M22" s="2"/>
     </row>
     <row r="23" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="26" t="s">
+      <c r="F23" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
     </row>
     <row r="24" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C24" s="24"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
     </row>
     <row r="25" spans="3:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2329,32 +2329,32 @@
       </c>
     </row>
     <row r="31" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C31" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
+      <c r="C31" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
     </row>
     <row r="32" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
     </row>
     <row r="35" spans="3:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" s="11" t="s">
@@ -2366,35 +2366,35 @@
       <c r="E35" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F35" s="32" t="s">
+      <c r="F35" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="25"/>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="D36" s="25" t="s">
+      <c r="D36" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="E36" s="24" t="s">
+      <c r="E36" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F36" s="26" t="s">
+      <c r="F36" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C37" s="24"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C39" s="9" t="s">
@@ -2437,32 +2437,32 @@
       </c>
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C44" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
+      <c r="C44" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="23"/>
     </row>
     <row r="45" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="21"/>
-      <c r="H45" s="21"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="23"/>
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C47" s="22" t="s">
+      <c r="C47" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D47" s="22"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="22"/>
-      <c r="G47" s="22"/>
-      <c r="H47" s="22"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="24"/>
     </row>
     <row r="48" spans="3:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C48" s="11" t="s">
@@ -2474,35 +2474,35 @@
       <c r="E48" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F48" s="32" t="s">
+      <c r="F48" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="G48" s="32"/>
-      <c r="H48" s="32"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="25"/>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C49" s="24" t="s">
+      <c r="C49" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D49" s="25" t="s">
+      <c r="D49" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="E49" s="24" t="s">
+      <c r="E49" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="26" t="s">
+      <c r="F49" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
+      <c r="G49" s="28"/>
+      <c r="H49" s="28"/>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C50" s="24"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="26"/>
-      <c r="H50" s="26"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="28"/>
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C52" s="9" t="s">
@@ -2545,32 +2545,32 @@
       </c>
     </row>
     <row r="57" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C57" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="D57" s="21"/>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
-      <c r="G57" s="21"/>
-      <c r="H57" s="21"/>
+      <c r="C57" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="23"/>
+      <c r="H57" s="23"/>
     </row>
     <row r="58" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
-      <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
-      <c r="G58" s="21"/>
-      <c r="H58" s="21"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
+      <c r="H58" s="23"/>
     </row>
     <row r="60" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C60" s="22" t="s">
+      <c r="C60" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D60" s="22"/>
-      <c r="E60" s="22"/>
-      <c r="F60" s="22"/>
-      <c r="G60" s="22"/>
-      <c r="H60" s="22"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="24"/>
+      <c r="H60" s="24"/>
     </row>
     <row r="61" spans="3:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C61" s="17" t="s">
@@ -2582,35 +2582,35 @@
       <c r="E61" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F61" s="32" t="s">
+      <c r="F61" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="G61" s="32"/>
-      <c r="H61" s="32"/>
+      <c r="G61" s="25"/>
+      <c r="H61" s="25"/>
     </row>
     <row r="62" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C62" s="24" t="s">
+      <c r="C62" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D62" s="25" t="s">
+      <c r="D62" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="E62" s="24" t="s">
+      <c r="E62" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F62" s="26" t="s">
+      <c r="F62" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G62" s="26"/>
-      <c r="H62" s="26"/>
+      <c r="G62" s="28"/>
+      <c r="H62" s="28"/>
     </row>
     <row r="63" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C63" s="24"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="24"/>
-      <c r="F63" s="26"/>
-      <c r="G63" s="26"/>
-      <c r="H63" s="26"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="27"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="28"/>
+      <c r="G63" s="28"/>
+      <c r="H63" s="28"/>
     </row>
     <row r="65" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C65" s="19" t="s">
@@ -2640,7 +2640,7 @@
         <v>39</v>
       </c>
       <c r="E66" s="14" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="F66" s="14" t="s">
         <v>40</v>
@@ -2692,6 +2692,7 @@
     <mergeCell ref="F49:H50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2713,117 +2714,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+    </row>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-    </row>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-    </row>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="31" t="s">
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="33" t="s">
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+    </row>
+    <row r="9" spans="3:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-    </row>
-    <row r="9" spans="3:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="35" t="s">
+      <c r="D10" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="36"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C13" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>80</v>
-      </c>
       <c r="E13" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F13" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="G13" s="19" t="s">
-        <v>85</v>
-      </c>
       <c r="H13" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="3:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2831,18 +2832,18 @@
         <v>14</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="H14" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="H14" s="22" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2858,5 +2859,225 @@
     <mergeCell ref="F10:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=_xmlsignatures/sig1.xml><?xml version="1.0" encoding="utf-8"?>
+<Signature xmlns="http://www.w3.org/2000/09/xmldsig#" Id="idPackageSignature">
+  <SignedInfo>
+    <CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315"/>
+    <SignatureMethod Algorithm="http://www.w3.org/2001/04/xmldsig-more#rsa-sha256"/>
+    <Reference Type="http://www.w3.org/2000/09/xmldsig#Object" URI="#idPackageObject">
+      <DigestMethod Algorithm="http://www.w3.org/2001/04/xmlenc#sha256"/>
+      <DigestValue>ZTZwzDiPkKAcqcapRJdFslbTDQvouqNOcDscfc3tx/4=</DigestValue>
+    </Reference>
+    <Reference Type="http://www.w3.org/2000/09/xmldsig#Object" URI="#idOfficeObject">
+      <DigestMethod Algorithm="http://www.w3.org/2001/04/xmlenc#sha256"/>
+      <DigestValue>JjJrH3UmlaprsVtRoxAmnMFsde0rNUGGzVUuyaonPGg=</DigestValue>
+    </Reference>
+    <Reference Type="http://uri.etsi.org/01903#SignedProperties" URI="#idSignedProperties">
+      <Transforms>
+        <Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315"/>
+      </Transforms>
+      <DigestMethod Algorithm="http://www.w3.org/2001/04/xmlenc#sha256"/>
+      <DigestValue>V4vraIKkycUiiJTCwqx8lmtyOThrZ2wlOsC2UzCywQo=</DigestValue>
+    </Reference>
+  </SignedInfo>
+  <SignatureValue>2z/Yj0+f1LbfKOaDXquZo1XqrDFE/NdpUeyXvi3xS26A2GYO/rCEZTYhLKjsOpgtsEyyzOb9TjOg
+sYHr0eT9t6KfV+4HbFdDNjqODVFRIhE/jYI/lKzZk48ih8mM7YXk0SIPpiKoowJXP4QBgFl3r9Xq
+qeSliageiF54bSLfP/aEXahEa7tkINzl/KMiIMi5107rcKFk7+VjNPXDyDslvj6XJhqLXWARjHKr
+3foCZuDUOVHtIvxSvBzW/DkasfNE3k5MK2J1SofPgNqTut/YOlwEK573muCvurKINhSlYZXuxtwi
+talh0fX1EaeWW7ZUjL2owC3FbX9l7vNbgFKVhQ==</SignatureValue>
+  <KeyInfo>
+    <X509Data>
+      <X509Certificate>MIID8jCCAtqgAwIBAgIQnV75Egz3ibRPF2VKDv8W6TANBgkqhkiG9w0BAQsFADB4MXYwEQYKCZImiZPyLGQBGRYDbmV0MBUGCgmSJomT8ixkARkWB3dpbmRvd3MwHQYDVQQDExZNUy1Pcmdhbml6YXRpb24tQWNjZXNzMCsGA1UECxMkODJkYmFjYTQtM2U4MS00NmNhLTljNzMtMDk1MGMxZWFjYTk3MB4XDTIxMTIxMTA3MjkyMloXDTMxMTIxMTA3NTkyMlowLzEtMCsGA1UEAxMkMmE4ZjlmYTYtYzExMS00ODQyLTk5YWItOTQzZmQyMWVlOWU2MIIBIjANBgkqhkiG9w0BAQEFAAOCAQ8AMIIBCgKCAQEA3kVbILCzyBpL4FGl3Tqr2JkKkrOTHgUpZU2Zqcim0V7NgtAy0orpLIYYX4iwVm2WrUNt1brS25pGGEOTH1mJyGVLPwlt1akv8t0PUc+1IpMskGmsN2ZziBdENI/ZtIXsWviBZO0KwOXWSyO50iUHLjiKUhp1xOZ36MQo9yhZRX2eFFr9cZrGzJ5w26mvvtQZsL0QcX3FjvdCoxiGrtqT4wEEUPjsaicLbEVHCbV8d0JbgYVNih81nsp7rgRoRB5HCT6XglPJwtzvk8D4kSbs3Wxxz7KtD4bYiqq0eRhuyTRGPDnZTUXdOdTF2y3MJGIERZNYrWmnsCDQEyQ2jfPcywIDAQABo4HAMIG9MAwGA1UdEwEB/wQCMAAwFgYDVR0lAQH/BAwwCgYIKwYBBQUHAwIwIgYLKoZIhvcUAQWCHAIEEwSBEKafjyoRwUJImauUP9Ie6eYwIgYLKoZIhvcUAQWCHAMEEwSBEFbmRIjtiyBMvQnhpyK8hSIwIgYLKoZIhvcUAQWCHAUEEwSBEEv9bF7TEqRLjqkZ2xlavaQwFAYLKoZIhvcUAQWCHAgEBQSBAkVVMBMGCyqGSIb3FAEFghwHBAQEgQEwMA0GCSqGSIb3DQEBCwUAA4IBAQBz595nI0QaX+sHYe2kLBWz3QGYjMwjVhaHIbeYaZxaHdV/NfE7EiJENh57c61DByX4Qfk1McMSXrRdDYqpEBoP/oMtl13bzcdul4HBtpeljIst0uDSvxKN4l9Htdlsh+JvGD5uwcUVtp7gD75Cm7xW8+PxlSPY86FIQREhsWM7pjA5h6/VkG126uldKhzK86roFcdUKPhbG5MVx0x+F/4H3uONW3RRCfbvzVro/e9l89jtX2WugQ96pJUDPlEOiGXkxoYsEJZiKfSBMv6osg67abyVBnVm2ryRcvlSb29EkVSPK/mB7PTSeO6fSMrv6/ylB/HFSqC7600MiXgSprX/</X509Certificate>
+    </X509Data>
+  </KeyInfo>
+  <Object Id="idPackageObject">
+    <Manifest>
+      <Reference URI="/_rels/.rels?ContentType=application/vnd.openxmlformats-package.relationships+xml">
+        <Transforms>
+          <Transform Algorithm="http://schemas.openxmlformats.org/package/2006/RelationshipTransform">
+            <mdssi:RelationshipReference xmlns:mdssi="http://schemas.openxmlformats.org/package/2006/digital-signature" SourceId="rId1"/>
+          </Transform>
+          <Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315"/>
+        </Transforms>
+        <DigestMethod Algorithm="http://www.w3.org/2001/04/xmlenc#sha256"/>
+        <DigestValue>2f3AFpmV4xMG5w1iTrxxA0J9QIy47+YsQamqbXmHTzc=</DigestValue>
+      </Reference>
+      <Reference URI="/xl/_rels/workbook.xml.rels?ContentType=application/vnd.openxmlformats-package.relationships+xml">
+        <Transforms>
+          <Transform Algorithm="http://schemas.openxmlformats.org/package/2006/RelationshipTransform">
+            <mdssi:RelationshipReference xmlns:mdssi="http://schemas.openxmlformats.org/package/2006/digital-signature" SourceId="rId3"/>
+            <mdssi:RelationshipReference xmlns:mdssi="http://schemas.openxmlformats.org/package/2006/digital-signature" SourceId="rId7"/>
+            <mdssi:RelationshipReference xmlns:mdssi="http://schemas.openxmlformats.org/package/2006/digital-signature" SourceId="rId2"/>
+            <mdssi:RelationshipReference xmlns:mdssi="http://schemas.openxmlformats.org/package/2006/digital-signature" SourceId="rId1"/>
+            <mdssi:RelationshipReference xmlns:mdssi="http://schemas.openxmlformats.org/package/2006/digital-signature" SourceId="rId6"/>
+            <mdssi:RelationshipReference xmlns:mdssi="http://schemas.openxmlformats.org/package/2006/digital-signature" SourceId="rId5"/>
+            <mdssi:RelationshipReference xmlns:mdssi="http://schemas.openxmlformats.org/package/2006/digital-signature" SourceId="rId4"/>
+          </Transform>
+          <Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315"/>
+        </Transforms>
+        <DigestMethod Algorithm="http://www.w3.org/2001/04/xmlenc#sha256"/>
+        <DigestValue>ZlWh0L0/tgVCKNwIdJCOZUeUEqiizbvBJduhJQ8maUc=</DigestValue>
+      </Reference>
+      <Reference URI="/xl/printerSettings/printerSettings1.bin?ContentType=application/vnd.openxmlformats-officedocument.spreadsheetml.printerSettings">
+        <DigestMethod Algorithm="http://www.w3.org/2001/04/xmlenc#sha256"/>
+        <DigestValue>BzQVw2H8Yuthgn1jcfPFZ+KfpYmS8hjGjIiVPQJ8YsA=</DigestValue>
+      </Reference>
+      <Reference URI="/xl/printerSettings/printerSettings2.bin?ContentType=application/vnd.openxmlformats-officedocument.spreadsheetml.printerSettings">
+        <DigestMethod Algorithm="http://www.w3.org/2001/04/xmlenc#sha256"/>
+        <DigestValue>BzQVw2H8Yuthgn1jcfPFZ+KfpYmS8hjGjIiVPQJ8YsA=</DigestValue>
+      </Reference>
+      <Reference URI="/xl/printerSettings/printerSettings3.bin?ContentType=application/vnd.openxmlformats-officedocument.spreadsheetml.printerSettings">
+        <DigestMethod Algorithm="http://www.w3.org/2001/04/xmlenc#sha256"/>
+        <DigestValue>BzQVw2H8Yuthgn1jcfPFZ+KfpYmS8hjGjIiVPQJ8YsA=</DigestValue>
+      </Reference>
+      <Reference URI="/xl/printerSettings/printerSettings4.bin?ContentType=application/vnd.openxmlformats-officedocument.spreadsheetml.printerSettings">
+        <DigestMethod Algorithm="http://www.w3.org/2001/04/xmlenc#sha256"/>
+        <DigestValue>BzQVw2H8Yuthgn1jcfPFZ+KfpYmS8hjGjIiVPQJ8YsA=</DigestValue>
+      </Reference>
+      <Reference URI="/xl/sharedStrings.xml?ContentType=application/vnd.openxmlformats-officedocument.spreadsheetml.sharedStrings+xml">
+        <DigestMethod Algorithm="http://www.w3.org/2001/04/xmlenc#sha256"/>
+        <DigestValue>WtvlF0LMhL/XUTt1FkixcyIlOiki5c7RyjZITdFBYiU=</DigestValue>
+      </Reference>
+      <Reference URI="/xl/styles.xml?ContentType=application/vnd.openxmlformats-officedocument.spreadsheetml.styles+xml">
+        <DigestMethod Algorithm="http://www.w3.org/2001/04/xmlenc#sha256"/>
+        <DigestValue>SpqDWaIr82BNL00EaxWAMmn/4j/9EUUaW+WwXjjCIUw=</DigestValue>
+      </Reference>
+      <Reference URI="/xl/theme/theme1.xml?ContentType=application/vnd.openxmlformats-officedocument.theme+xml">
+        <DigestMethod Algorithm="http://www.w3.org/2001/04/xmlenc#sha256"/>
+        <DigestValue>5gKatJWEFLi7hisX/+06cI0VE+YaB9iOlmBxzKMdG9Q=</DigestValue>
+      </Reference>
+      <Reference URI="/xl/workbook.xml?ContentType=application/vnd.openxmlformats-officedocument.spreadsheetml.sheet.main+xml">
+        <DigestMethod Algorithm="http://www.w3.org/2001/04/xmlenc#sha256"/>
+        <DigestValue>V7PJCLXXltQZhzXLKEU7TjaLgXPLgcGjWDfN5a3FWMA=</DigestValue>
+      </Reference>
+      <Reference URI="/xl/worksheets/_rels/sheet1.xml.rels?ContentType=application/vnd.openxmlformats-package.relationships+xml">
+        <Transforms>
+          <Transform Algorithm="http://schemas.openxmlformats.org/package/2006/RelationshipTransform">
+            <mdssi:RelationshipReference xmlns:mdssi="http://schemas.openxmlformats.org/package/2006/digital-signature" SourceId="rId1"/>
+          </Transform>
+          <Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315"/>
+        </Transforms>
+        <DigestMethod Algorithm="http://www.w3.org/2001/04/xmlenc#sha256"/>
+        <DigestValue>DFvVPqoIk86WVQiP0UyA3uzCQioz46PDY/dKih+lBrk=</DigestValue>
+      </Reference>
+      <Reference URI="/xl/worksheets/_rels/sheet2.xml.rels?ContentType=application/vnd.openxmlformats-package.relationships+xml">
+        <Transforms>
+          <Transform Algorithm="http://schemas.openxmlformats.org/package/2006/RelationshipTransform">
+            <mdssi:RelationshipReference xmlns:mdssi="http://schemas.openxmlformats.org/package/2006/digital-signature" SourceId="rId1"/>
+          </Transform>
+          <Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315"/>
+        </Transforms>
+        <DigestMethod Algorithm="http://www.w3.org/2001/04/xmlenc#sha256"/>
+        <DigestValue>ie1t59T+oh4xR4rir291kA0PxL5MlUFD/HEFvVUbc9Y=</DigestValue>
+      </Reference>
+      <Reference URI="/xl/worksheets/_rels/sheet3.xml.rels?ContentType=application/vnd.openxmlformats-package.relationships+xml">
+        <Transforms>
+          <Transform Algorithm="http://schemas.openxmlformats.org/package/2006/RelationshipTransform">
+            <mdssi:RelationshipReference xmlns:mdssi="http://schemas.openxmlformats.org/package/2006/digital-signature" SourceId="rId1"/>
+          </Transform>
+          <Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315"/>
+        </Transforms>
+        <DigestMethod Algorithm="http://www.w3.org/2001/04/xmlenc#sha256"/>
+        <DigestValue>QSYMNFtFM/We0x/y91OmLCZOt/Fg9jrJRLrG/1nsbrY=</DigestValue>
+      </Reference>
+      <Reference URI="/xl/worksheets/_rels/sheet4.xml.rels?ContentType=application/vnd.openxmlformats-package.relationships+xml">
+        <Transforms>
+          <Transform Algorithm="http://schemas.openxmlformats.org/package/2006/RelationshipTransform">
+            <mdssi:RelationshipReference xmlns:mdssi="http://schemas.openxmlformats.org/package/2006/digital-signature" SourceId="rId1"/>
+          </Transform>
+          <Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315"/>
+        </Transforms>
+        <DigestMethod Algorithm="http://www.w3.org/2001/04/xmlenc#sha256"/>
+        <DigestValue>Auuqa0XyaXU4hdxM770k/DVyj5HFS3KFPVMKRz5ysj0=</DigestValue>
+      </Reference>
+      <Reference URI="/xl/worksheets/sheet1.xml?ContentType=application/vnd.openxmlformats-officedocument.spreadsheetml.worksheet+xml">
+        <DigestMethod Algorithm="http://www.w3.org/2001/04/xmlenc#sha256"/>
+        <DigestValue>gR8ONbf5pKd6nhsCtZ6K/hpoKCxt5ilqinOr3fhJ6H8=</DigestValue>
+      </Reference>
+      <Reference URI="/xl/worksheets/sheet2.xml?ContentType=application/vnd.openxmlformats-officedocument.spreadsheetml.worksheet+xml">
+        <DigestMethod Algorithm="http://www.w3.org/2001/04/xmlenc#sha256"/>
+        <DigestValue>5rXA6Cbq15jeaHsNieHLGXvOjxBbKN/4nmTjnhBbnxk=</DigestValue>
+      </Reference>
+      <Reference URI="/xl/worksheets/sheet3.xml?ContentType=application/vnd.openxmlformats-officedocument.spreadsheetml.worksheet+xml">
+        <DigestMethod Algorithm="http://www.w3.org/2001/04/xmlenc#sha256"/>
+        <DigestValue>0JGpvK4t0IiCCeDJY/yt/PQRhAUeJBXiDaZCM3nn7X4=</DigestValue>
+      </Reference>
+      <Reference URI="/xl/worksheets/sheet4.xml?ContentType=application/vnd.openxmlformats-officedocument.spreadsheetml.worksheet+xml">
+        <DigestMethod Algorithm="http://www.w3.org/2001/04/xmlenc#sha256"/>
+        <DigestValue>iTEs6pDM52hbbNNw5IojQwA4AK0YDykaj+SP5cJMJmw=</DigestValue>
+      </Reference>
+    </Manifest>
+    <SignatureProperties>
+      <SignatureProperty Id="idSignatureTime" Target="#idPackageSignature">
+        <mdssi:SignatureTime xmlns:mdssi="http://schemas.openxmlformats.org/package/2006/digital-signature">
+          <mdssi:Format>YYYY-MM-DDThh:mm:ssTZD</mdssi:Format>
+          <mdssi:Value>2022-05-15T09:02:42Z</mdssi:Value>
+        </mdssi:SignatureTime>
+      </SignatureProperty>
+    </SignatureProperties>
+  </Object>
+  <Object Id="idOfficeObject">
+    <SignatureProperties>
+      <SignatureProperty Id="idOfficeV1Details" Target="#idPackageSignature">
+        <SignatureInfoV1 xmlns="http://schemas.microsoft.com/office/2006/digsig">
+          <SetupID/>
+          <SignatureText/>
+          <SignatureImage/>
+          <SignatureComments>Copyright</SignatureComments>
+          <WindowsVersion>10.0</WindowsVersion>
+          <OfficeVersion>16.0</OfficeVersion>
+          <ApplicationVersion>16.0</ApplicationVersion>
+          <Monitors>2</Monitors>
+          <HorizontalResolution>1920</HorizontalResolution>
+          <VerticalResolution>1080</VerticalResolution>
+          <ColorDepth>32</ColorDepth>
+          <SignatureProviderId>{00000000-0000-0000-0000-000000000000}</SignatureProviderId>
+          <SignatureProviderUrl/>
+          <SignatureProviderDetails>9</SignatureProviderDetails>
+          <SignatureType>1</SignatureType>
+        </SignatureInfoV1>
+      </SignatureProperty>
+    </SignatureProperties>
+  </Object>
+  <Object>
+    <xd:QualifyingProperties xmlns:xd="http://uri.etsi.org/01903/v1.3.2#" Target="#idPackageSignature">
+      <xd:SignedProperties Id="idSignedProperties">
+        <xd:SignedSignatureProperties>
+          <xd:SigningTime>2022-05-15T09:02:42Z</xd:SigningTime>
+          <xd:SigningCertificate>
+            <xd:Cert>
+              <xd:CertDigest>
+                <DigestMethod Algorithm="http://www.w3.org/2001/04/xmlenc#sha256"/>
+                <DigestValue>0UOHHDvFzuOaFRQV0/J7Uw60vPSV8HpfqJwbOFmgQAc=</DigestValue>
+              </xd:CertDigest>
+              <xd:IssuerSerial>
+                <X509IssuerName>DC=net + DC=windows + CN=MS-Organization-Access + OU=82dbaca4-3e81-46ca-9c73-0950c1eaca97</X509IssuerName>
+                <X509SerialNumber>209181922993045375451295390530499712745</X509SerialNumber>
+              </xd:IssuerSerial>
+            </xd:Cert>
+          </xd:SigningCertificate>
+          <xd:SignaturePolicyIdentifier>
+            <xd:SignaturePolicyImplied/>
+          </xd:SignaturePolicyIdentifier>
+        </xd:SignedSignatureProperties>
+        <xd:SignedDataObjectProperties>
+          <xd:CommitmentTypeIndication>
+            <xd:CommitmentTypeId>
+              <xd:Identifier>http://uri.etsi.org/01903/v1.2.2#ProofOfCreation</xd:Identifier>
+              <xd:Description>Created this document</xd:Description>
+            </xd:CommitmentTypeId>
+            <xd:AllSignedDataObjects/>
+            <xd:CommitmentTypeQualifiers>
+              <xd:CommitmentTypeQualifier>Copyright</xd:CommitmentTypeQualifier>
+            </xd:CommitmentTypeQualifiers>
+          </xd:CommitmentTypeIndication>
+        </xd:SignedDataObjectProperties>
+      </xd:SignedProperties>
+    </xd:QualifyingProperties>
+  </Object>
+</Signature>
 </file>
</xml_diff>